<commit_message>
Add unfinished CAD model
</commit_message>
<xml_diff>
--- a/Gears_Measurements.xlsx
+++ b/Gears_Measurements.xlsx
@@ -47,10 +47,10 @@
     <t>Pitch</t>
   </si>
   <si>
-    <t>Primitive Diameter</t>
-  </si>
-  <si>
     <t>Foot Diameter</t>
+  </si>
+  <si>
+    <t>Primitive Diameter/ Base Circle</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,42 +408,74 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>29.75</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <f>B2/(A2+2)</f>
-        <v>1.3522727272727273</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>1/C2</f>
-        <v>0.73949579831932777</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f>A2/D2</f>
-        <v>27.045454545454543</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <f>C2*PI()</f>
-        <v>4.2482900656498339</v>
+        <v>3.1415926535897931</v>
       </c>
       <c r="G2">
         <f>C2*A2</f>
-        <v>27.045454545454547</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <f>G2-2*C2</f>
-        <v>24.340909090909093</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <f>B3/(A3+2)</f>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f>1/C3</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>A3/D3</f>
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <f>C3*PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G3">
+        <f>C3*A3</f>
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <f>G3-2*C3</f>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>